<commit_message>
added files to DOE
</commit_message>
<xml_diff>
--- a/DOE/katoen.xlsx
+++ b/DOE/katoen.xlsx
@@ -1,14 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A0CFA38E-F76F-4141-9477-DEE63C4A7D0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lteeg\Documents\Github\School\DOE\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A77B606-7F16-44E0-9193-5F363C835C33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
+    <sheet name="Blad2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -28,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>15%</t>
   </si>
@@ -43,13 +49,37 @@
   </si>
   <si>
     <t>35%</t>
+  </si>
+  <si>
+    <t>katoen percentage</t>
+  </si>
+  <si>
+    <t>observations</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>treatment</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -57,13 +87,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -75,17 +117,41 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Accent1" xfId="1" builtinId="29"/>
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -98,8 +164,30 @@
 </styleSheet>
 </file>
 
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{69F38421-8695-471E-8EAA-D6C2A3B022CB}" name="Tabel3" displayName="Tabel3" ref="A2:F7" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A2:F7" xr:uid="{69F38421-8695-471E-8EAA-D6C2A3B022CB}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{7ACBBCC4-2BC9-496B-9521-5C7751EB52A2}" name="treatment" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{B210010E-F67A-4636-9575-BAB5E29C4B23}" name="1"/>
+    <tableColumn id="3" xr3:uid="{0616D8F0-77DB-4D9B-8A47-93128CE7FABD}" name="2"/>
+    <tableColumn id="4" xr3:uid="{5133D60D-D326-41DF-B2C6-16A81E286915}" name="3"/>
+    <tableColumn id="5" xr3:uid="{B562368A-6FBD-445A-9191-15EE5F2A30E1}" name="4"/>
+    <tableColumn id="6" xr3:uid="{F57EE9DC-7F9B-426C-9457-94FA0E0C6EF3}" name="5"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -397,13 +485,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -420,7 +508,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>7</v>
       </c>
@@ -437,7 +525,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>7</v>
       </c>
@@ -454,7 +542,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>15</v>
       </c>
@@ -471,7 +559,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>11</v>
       </c>
@@ -488,7 +576,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>9</v>
       </c>
@@ -508,4 +596,163 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B28DD0F-E9DB-42AC-B2A3-D08E667D8E8D}">
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>15</v>
+      </c>
+      <c r="B3" s="2">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2">
+        <v>7</v>
+      </c>
+      <c r="D3" s="2">
+        <v>15</v>
+      </c>
+      <c r="E3" s="2">
+        <v>11</v>
+      </c>
+      <c r="F3" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>20</v>
+      </c>
+      <c r="B4" s="2">
+        <v>12</v>
+      </c>
+      <c r="C4" s="2">
+        <v>17</v>
+      </c>
+      <c r="D4" s="2">
+        <v>12</v>
+      </c>
+      <c r="E4" s="2">
+        <v>18</v>
+      </c>
+      <c r="F4" s="2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>25</v>
+      </c>
+      <c r="B5" s="2">
+        <v>14</v>
+      </c>
+      <c r="C5" s="2">
+        <v>18</v>
+      </c>
+      <c r="D5" s="2">
+        <v>18</v>
+      </c>
+      <c r="E5" s="2">
+        <v>19</v>
+      </c>
+      <c r="F5" s="2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>30</v>
+      </c>
+      <c r="B6" s="2">
+        <v>19</v>
+      </c>
+      <c r="C6" s="2">
+        <v>25</v>
+      </c>
+      <c r="D6" s="2">
+        <v>22</v>
+      </c>
+      <c r="E6" s="2">
+        <v>19</v>
+      </c>
+      <c r="F6" s="2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>35</v>
+      </c>
+      <c r="B7" s="2">
+        <v>7</v>
+      </c>
+      <c r="C7" s="2">
+        <v>10</v>
+      </c>
+      <c r="D7" s="2">
+        <v>11</v>
+      </c>
+      <c r="E7" s="2">
+        <v>15</v>
+      </c>
+      <c r="F7" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>